<commit_message>
Changed bar graph and made minor fixed on the references
</commit_message>
<xml_diff>
--- a/tex/dados_pesquisa_lang_apda.xlsx
+++ b/tex/dados_pesquisa_lang_apda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23250" windowHeight="13290"/>
+    <workbookView windowWidth="28695" windowHeight="13245"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -75,12 +75,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -89,10 +89,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -101,6 +110,28 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -113,23 +144,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,9 +158,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,37 +175,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,7 +204,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,31 +212,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -249,187 +242,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,6 +433,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -468,16 +476,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,21 +510,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -527,16 +520,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,156 +538,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -703,15 +693,15 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="2" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="6" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="7" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="8" builtinId="43"/>
-    <cellStyle name="60% - Accent3" xfId="9" builtinId="40"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
     <cellStyle name="Accent4" xfId="10" builtinId="41"/>
     <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
     <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
@@ -720,37 +710,37 @@
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
     <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="Porcentagem" xfId="18" builtinId="5"/>
-    <cellStyle name="40% - Accent1" xfId="19" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="21" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="22" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="23" builtinId="32"/>
-    <cellStyle name="Bad" xfId="24" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="25" builtinId="42"/>
-    <cellStyle name="20% - Accent3" xfId="26" builtinId="38"/>
-    <cellStyle name="Moeda" xfId="27" builtinId="4"/>
-    <cellStyle name="Check Cell" xfId="28" builtinId="23"/>
-    <cellStyle name="Good" xfId="29" builtinId="26"/>
-    <cellStyle name="Calculation" xfId="30" builtinId="22"/>
-    <cellStyle name="Total" xfId="31" builtinId="25"/>
-    <cellStyle name="Output" xfId="32" builtinId="21"/>
-    <cellStyle name="60% - Accent6" xfId="33" builtinId="52"/>
-    <cellStyle name="Hyperlink seguido" xfId="34" builtinId="9"/>
-    <cellStyle name="Moeda [0]" xfId="35" builtinId="7"/>
-    <cellStyle name="Note" xfId="36" builtinId="10"/>
-    <cellStyle name="Input" xfId="37" builtinId="20"/>
-    <cellStyle name="Heading 3" xfId="38" builtinId="18"/>
-    <cellStyle name="Heading 1" xfId="39" builtinId="16"/>
-    <cellStyle name="CExplanatory Text" xfId="40" builtinId="53"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Comma [0]" xfId="42" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="43" builtinId="50"/>
-    <cellStyle name="Title" xfId="44" builtinId="15"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
     <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
     <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Heading 4" xfId="47" builtinId="19"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -970,7 +960,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:rPr>
-                  <a:t>Linguagens de Programação</a:t>
+                  <a:t>Linguagens de programação</a:t>
                 </a:r>
                 <a:endParaRPr lang="x-none" altLang="pt-BR" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
                   <a:solidFill>
@@ -1080,7 +1070,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:rPr>
-                  <a:t>Quantidade de utilizadores como linguagem de introdução à programação</a:t>
+                  <a:t>Quantidade de usuários</a:t>
                 </a:r>
                 <a:endParaRPr lang="x-none" altLang="pt-BR" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
                   <a:solidFill>
@@ -2034,7 +2024,7 @@
   <dimension ref="B13:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2054,18 +2044,18 @@
       </c>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>570</v>
       </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>169</v>
       </c>
       <c r="H15" t="s">
@@ -2074,16 +2064,16 @@
       <c r="I15">
         <v>570</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <f>I15/$I$29</f>
         <v>0.55019305019305</v>
       </c>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>122</v>
       </c>
       <c r="H16" t="s">
@@ -2092,16 +2082,16 @@
       <c r="I16">
         <v>169</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <f t="shared" ref="J16:J27" si="0">I16/$I$29</f>
         <v>0.163127413127413</v>
       </c>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>64</v>
       </c>
       <c r="H17" t="s">
@@ -2110,16 +2100,16 @@
       <c r="I17">
         <v>122</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <f t="shared" si="0"/>
         <v>0.117760617760618</v>
       </c>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>56</v>
       </c>
       <c r="H18" t="s">
@@ -2128,16 +2118,16 @@
       <c r="I18">
         <v>64</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <f t="shared" si="0"/>
         <v>0.0617760617760618</v>
       </c>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>55</v>
       </c>
       <c r="H19" t="s">
@@ -2146,105 +2136,91 @@
       <c r="I19">
         <v>56</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <f t="shared" si="0"/>
         <v>0.0540540540540541</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+    <row r="20" spans="8:10">
       <c r="H20" t="s">
         <v>9</v>
       </c>
       <c r="I20">
         <v>28</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <f t="shared" si="0"/>
         <v>0.027027027027027</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+    <row r="21" spans="8:10">
       <c r="H21" t="s">
         <v>10</v>
       </c>
       <c r="I21">
         <v>12</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
         <f t="shared" si="0"/>
         <v>0.0115830115830116</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+    <row r="22" spans="8:10">
       <c r="H22" t="s">
         <v>11</v>
       </c>
       <c r="I22">
         <v>9</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
         <f t="shared" si="0"/>
         <v>0.00868725868725869</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+    <row r="23" spans="8:10">
       <c r="H23" t="s">
         <v>12</v>
       </c>
       <c r="I23">
         <v>2</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="1">
         <f t="shared" si="0"/>
         <v>0.00193050193050193</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+    <row r="24" spans="8:10">
       <c r="H24" t="s">
         <v>13</v>
       </c>
       <c r="I24">
         <v>2</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="1">
         <f t="shared" si="0"/>
         <v>0.00193050193050193</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+    <row r="25" spans="8:10">
       <c r="H25" t="s">
         <v>14</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <f t="shared" si="0"/>
         <v>0.000965250965250965</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+    <row r="26" spans="8:10">
       <c r="H26" t="s">
         <v>15</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="1">
         <f t="shared" si="0"/>
         <v>0.000965250965250965</v>
       </c>
@@ -2256,7 +2232,7 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2269,7 +2245,7 @@
         <f>SUM(I15:I27)</f>
         <v>1036</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <f>SUM(J15:J27)</f>
         <v>1</v>
       </c>

</xml_diff>